<commit_message>
May extra edits 2
Extra edits code: K reduction fouling extensions, full-scale simulations
</commit_message>
<xml_diff>
--- a/7.1_Extending_the_USEPA_fouling_approach/7.1_Input_PFHpA.xlsx
+++ b/7.1_Extending_the_USEPA_fouling_approach/7.1_Input_PFHpA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\PycharmProjects\Thesis-Activated-Carbon-Modelling\1USEPA_PSDM\7PSDM_EditMathieu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\PycharmProjects\Thesis-Modelling-activated-carbon\7.1_Extending_the_USEPA_fouling_approach\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D352D5-4066-4540-B80E-5390F725191A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8100C32A-2DFE-418E-9867-2B834643559F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{317BF3F6-A68C-4964-9BC3-AEDC7E3058F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="1" r:id="rId1"/>
@@ -637,18 +637,18 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -656,7 +656,7 @@
         <v>364.06</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -664,7 +664,7 @@
         <v>203.15799999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -672,7 +672,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -680,7 +680,7 @@
         <v>1.792</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -688,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -704,7 +704,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -712,7 +712,7 @@
         <v>5.52</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -720,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -728,7 +728,7 @@
         <v>13.83</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -745,18 +745,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB297697-1B90-46DD-B82E-FCE20BA48421}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -764,7 +764,7 @@
         <v>6.7640000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -772,7 +772,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -780,7 +780,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -788,7 +788,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -809,12 +809,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -825,7 +825,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -833,7 +833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -844,7 +844,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -852,7 +852,7 @@
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -860,7 +860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -871,7 +871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -882,7 +882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -893,7 +893,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -904,7 +904,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -915,7 +915,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -926,7 +926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -934,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -942,7 +942,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -950,7 +950,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -958,7 +958,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
@@ -975,19 +975,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401BCFB4-DB77-4CE9-BB3A-E676947AF423}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1009,27 +1009,27 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>50000</v>
+        <v>0.04</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="C3">
-        <v>50000</v>
+        <v>0.04</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1043,12 +1043,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
       <c r="B5">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1070,15 +1070,15 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1259,18 +1259,18 @@
       <selection activeCell="A3" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="31.2" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="6"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="148" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="63" x14ac:dyDescent="0.5">
       <c r="B1" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:2" ht="63" x14ac:dyDescent="0.5">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:2" ht="63" x14ac:dyDescent="0.5">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="156" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" ht="157.5" x14ac:dyDescent="0.5">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:2" ht="94.5" x14ac:dyDescent="0.5">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:2" ht="63" x14ac:dyDescent="0.5">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:2" ht="63" x14ac:dyDescent="0.5">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -1331,15 +1331,15 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>

</xml_diff>